<commit_message>
Reformulação de entrada de arquivos para implementação de entry de aba. Implementação do entry de aba'
</commit_message>
<xml_diff>
--- a/Planejamento da GUI.xlsx
+++ b/Planejamento da GUI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Tipo de arquivo:</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Arquivo de dados:</t>
   </si>
   <si>
-    <t>________GRARED_P.xlsx_______</t>
-  </si>
-  <si>
     <t>Tabela de conversão:</t>
   </si>
   <si>
@@ -121,6 +118,15 @@
   </si>
   <si>
     <t>****Gerar Arquivos de Saída****</t>
+  </si>
+  <si>
+    <t>Aba da Planilha</t>
+  </si>
+  <si>
+    <t>______Plan1_____</t>
+  </si>
+  <si>
+    <t>_____GRARED_P.xlsx_____</t>
   </si>
 </sst>
 </file>
@@ -247,12 +253,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -261,11 +270,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,7 +581,7 @@
   <dimension ref="A1:AJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8:AC8"/>
+      <selection activeCell="U6" sqref="U6:AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
@@ -712,48 +718,48 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="5" t="s">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
     </row>
@@ -761,38 +767,42 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
     </row>
@@ -800,93 +810,93 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-    </row>
-    <row r="6" spans="1:36" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:36" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="6"/>
+      <c r="J6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="J6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="M6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="Q6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="U6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-    </row>
-    <row r="7" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="6"/>
+      <c r="M6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="Q6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="U6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+    </row>
+    <row r="7" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="M7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="Q7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="J7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="Q7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -898,118 +908,118 @@
       <c r="F8" s="2">
         <v>10</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="7">
         <v>2017</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="J8" s="5">
+      <c r="H8" s="7"/>
+      <c r="J8" s="7">
         <v>-3</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="M8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="Q8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="U8" s="8">
+      <c r="K8" s="7"/>
+      <c r="M8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="Q8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="U8" s="9">
         <v>980998.098</v>
       </c>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
+      <c r="M9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="I10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U10" s="9" t="s">
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Z10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="V10" s="9"/>
-      <c r="W10" s="9"/>
-      <c r="X10" s="9"/>
-      <c r="Z10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="5"/>
     </row>
     <row r="11" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
+      <c r="M11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
     </row>
     <row r="12" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1019,31 +1029,31 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S12" s="6"/>
+      <c r="T12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
     </row>
     <row r="13" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1053,17 +1063,17 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="M13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
+      <c r="M13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1114,7 +1124,31 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="38">
+    <mergeCell ref="X3:AC4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:S3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G6:H7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M5:U5"/>
+    <mergeCell ref="T3:W4"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="K12:P12"/>
+    <mergeCell ref="M11:U11"/>
+    <mergeCell ref="M2:U2"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="M9:U9"/>
+    <mergeCell ref="U10:X10"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="R12:S12"/>
     <mergeCell ref="T12:Y12"/>
@@ -1123,34 +1157,12 @@
     <mergeCell ref="U8:AC8"/>
     <mergeCell ref="AA10:AC10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="M11:U11"/>
-    <mergeCell ref="M2:U2"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:M4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="N3:S4"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="M9:U9"/>
-    <mergeCell ref="U10:X10"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="Q8:S8"/>
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="M7:O7"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G6:H7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="M5:U5"/>
-    <mergeCell ref="T3:W4"/>
-    <mergeCell ref="X3:AC4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalização da GUI. Término da adequação das transformações matemáticas à GUI. Mudanças finais da planilha de projeto da GUI. Início da implementação da saída de dados
</commit_message>
<xml_diff>
--- a/Planejamento da GUI.xlsx
+++ b/Planejamento da GUI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Tipo de arquivo:</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Densidade</t>
   </si>
   <si>
-    <t>Crust. g/cm^3</t>
-  </si>
-  <si>
     <t>2.67</t>
   </si>
   <si>
@@ -108,18 +105,9 @@
     <t>Saída Excel:</t>
   </si>
   <si>
-    <t>Levantamento_19_10_2017.txt</t>
-  </si>
-  <si>
     <t>SaídaTXT</t>
   </si>
   <si>
-    <t>Levantamento_19_10_2017.xlsx</t>
-  </si>
-  <si>
-    <t>****Gerar Arquivos de Saída****</t>
-  </si>
-  <si>
     <t>Aba da Planilha</t>
   </si>
   <si>
@@ -127,6 +115,45 @@
   </si>
   <si>
     <t>_____GRARED_P.xlsx_____</t>
+  </si>
+  <si>
+    <t>GRS67</t>
+  </si>
+  <si>
+    <t>GRS80</t>
+  </si>
+  <si>
+    <t>GRS84</t>
+  </si>
+  <si>
+    <t>Elipsóide de referência:</t>
+  </si>
+  <si>
+    <t>Crust. (cgs)</t>
+  </si>
+  <si>
+    <t>____980998,098___</t>
+  </si>
+  <si>
+    <t>_19_</t>
+  </si>
+  <si>
+    <t>_10_</t>
+  </si>
+  <si>
+    <t>_2017_</t>
+  </si>
+  <si>
+    <t>dados_reduzidos.txt</t>
+  </si>
+  <si>
+    <t>dados_reduzidos.xlsx</t>
+  </si>
+  <si>
+    <t>****Reduzir Dados e Gerar Saída***</t>
+  </si>
+  <si>
+    <t>Autoria do programa</t>
   </si>
 </sst>
 </file>
@@ -136,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +213,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -201,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -233,12 +266,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -255,11 +297,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -267,14 +324,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -578,16 +632,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:AC7"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="4.7109375" style="2"/>
+    <col min="2" max="17" width="4.7109375" style="2"/>
+    <col min="18" max="18" width="6.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="4.7109375" style="2"/>
+    <col min="20" max="20" width="6" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="4.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -702,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
@@ -718,48 +776,48 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="6" t="s">
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="7" t="s">
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
     </row>
@@ -767,42 +825,42 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
     </row>
@@ -810,17 +868,17 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
+      <c r="M5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
     </row>
     <row r="6" spans="1:36" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -828,41 +886,41 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="J6" s="6" t="s">
+      <c r="H6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="6"/>
-      <c r="M6" s="6" t="s">
+      <c r="K6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="Q6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="U6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="Q6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="U6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
     </row>
     <row r="7" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -870,212 +928,237 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="J7" s="6" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="M7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="Q7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
+      <c r="K7" s="9"/>
+      <c r="M7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="Q7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="E8" s="2">
-        <v>19</v>
-      </c>
-      <c r="F8" s="2">
-        <v>10</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2017</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="J8" s="7">
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="J8" s="8">
         <v>-3</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="M8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="Q8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="U8" s="9">
-        <v>980998.098</v>
-      </c>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
+      <c r="K8" s="8"/>
+      <c r="M8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="Q8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="U8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
+      <c r="M9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
       <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="5"/>
       <c r="N10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
       <c r="S10" s="5"/>
       <c r="T10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Z10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="10"/>
-      <c r="Z10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
       <c r="AD10" s="5"/>
     </row>
-    <row r="11" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-    </row>
-    <row r="12" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="8"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y11" s="8"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="5"/>
+    </row>
+    <row r="12" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-    </row>
-    <row r="13" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+    </row>
+    <row r="13" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="M13" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="H13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
+      <c r="Q13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="U13" s="8"/>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+    </row>
+    <row r="14" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1083,20 +1166,44 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="M14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="1:36" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="B15" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1123,21 +1230,35 @@
         <v>19</v>
       </c>
     </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="X3:AC4"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:S3"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G6:H7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="M5:U5"/>
-    <mergeCell ref="T3:W4"/>
+  <mergeCells count="43">
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="T13:Y13"/>
+    <mergeCell ref="M14:U14"/>
+    <mergeCell ref="U6:AC7"/>
+    <mergeCell ref="U8:AC8"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="Q13:S13"/>
     <mergeCell ref="D10:G10"/>
-    <mergeCell ref="K12:P12"/>
-    <mergeCell ref="M11:U11"/>
+    <mergeCell ref="K13:P13"/>
+    <mergeCell ref="M12:U12"/>
     <mergeCell ref="M2:U2"/>
     <mergeCell ref="B3:E4"/>
     <mergeCell ref="G3:I3"/>
@@ -1149,20 +1270,16 @@
     <mergeCell ref="Q6:S6"/>
     <mergeCell ref="Q7:S7"/>
     <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="T12:Y12"/>
-    <mergeCell ref="M13:U13"/>
-    <mergeCell ref="U6:AC7"/>
-    <mergeCell ref="U8:AC8"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G6:H7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M5:U5"/>
+    <mergeCell ref="T3:W4"/>
+    <mergeCell ref="X3:AC4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:S3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ver. ALpha0.5, Implementação da correção de maré, truncagem da saída em 3 casas decimais, retirada de fator grav, correção da leitura dos dados na planilha
</commit_message>
<xml_diff>
--- a/Planejamento da GUI.xlsx
+++ b/Planejamento da GUI.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Tipo de arquivo:</t>
   </si>
@@ -57,16 +57,7 @@
     <t>2.67</t>
   </si>
   <si>
-    <t>Fator</t>
-  </si>
-  <si>
-    <t>1.20</t>
-  </si>
-  <si>
     <t>Aceleração grav. da primeira estação (mGal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gravimétrico</t>
   </si>
   <si>
     <t>Escolha das correções</t>
@@ -300,32 +291,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -632,7 +623,7 @@
   <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,29 +747,29 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
+      <c r="M2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
       <c r="X2" s="3"/>
     </row>
     <row r="3" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
@@ -787,26 +778,26 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
       <c r="X3" s="11" t="s">
         <v>5</v>
       </c>
@@ -822,36 +813,36 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
-      <c r="J4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
+      <c r="J4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
@@ -865,17 +856,17 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
+      <c r="M5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
     </row>
     <row r="6" spans="1:36" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -883,41 +874,39 @@
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="12"/>
+      <c r="J6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="K6" s="12"/>
+      <c r="M6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="Q6" s="9" t="s">
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="U6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="U6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
     </row>
     <row r="7" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -925,46 +914,44 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="J7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="M7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="Q7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9"/>
-      <c r="Y7" s="9"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
+      <c r="K7" s="12"/>
+      <c r="M7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H8" s="11"/>
       <c r="J8" s="11">
@@ -976,13 +963,11 @@
       </c>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="Q8" s="11" t="s">
-        <v>14</v>
-      </c>
+      <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="U8" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
@@ -997,57 +982,57 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="M9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
+      <c r="M9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
       <c r="I10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
       <c r="M10" s="5"/>
       <c r="N10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="O10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
       <c r="S10" s="5"/>
       <c r="T10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
-      <c r="AA10" s="12"/>
-      <c r="AB10" s="12"/>
-      <c r="AC10" s="12"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
       <c r="AD10" s="5"/>
     </row>
     <row r="11" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1060,18 +1045,18 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="J11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q11" s="11"/>
       <c r="R11" s="7"/>
@@ -1079,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="U11" s="11"/>
       <c r="V11" s="7"/>
@@ -1087,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="X11" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Y11" s="11"/>
       <c r="AA11" s="7"/>
@@ -1099,17 +1084,17 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="M12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
+      <c r="M12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
     </row>
     <row r="13" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1118,26 +1103,26 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="H13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
+      <c r="Q13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
       <c r="T13" s="11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
@@ -1153,35 +1138,35 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="M14" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
+      <c r="M14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:36" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -1224,20 +1209,19 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="T13:Y13"/>
-    <mergeCell ref="M14:U14"/>
-    <mergeCell ref="U8:AC8"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="M5:U5"/>
+    <mergeCell ref="T3:W4"/>
+    <mergeCell ref="X3:AC4"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:S3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="U6:AC7"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="K13:P13"/>
     <mergeCell ref="M12:U12"/>
@@ -1254,19 +1238,20 @@
     <mergeCell ref="Q8:S8"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G6:H7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="M5:U5"/>
-    <mergeCell ref="T3:W4"/>
-    <mergeCell ref="X3:AC4"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:S3"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="U6:AC7"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="U8:AC8"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="T13:Y13"/>
+    <mergeCell ref="M14:U14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Lançamento da versão 1.0
</commit_message>
<xml_diff>
--- a/Planejamento da GUI.xlsx
+++ b/Planejamento da GUI.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t xml:space="preserve">Entrada dos dados</t>
   </si>
@@ -105,13 +105,10 @@
     <t xml:space="preserve">@</t>
   </si>
   <si>
-    <t xml:space="preserve">Free-Air</t>
+    <t xml:space="preserve">Free-air</t>
   </si>
   <si>
     <t xml:space="preserve">Bouguer Simples</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pressão Atmosférica</t>
   </si>
   <si>
     <t xml:space="preserve">Elipsóide de referência:</t>
@@ -438,7 +435,7 @@
   <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -809,7 +806,7 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -817,33 +814,22 @@
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="M10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
-      <c r="S10" s="11"/>
+      <c r="S10" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="T10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="U10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
+        <v>28</v>
+      </c>
       <c r="X10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
@@ -861,7 +847,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -871,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="12"/>
@@ -879,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U11" s="6"/>
       <c r="V11" s="12"/>
@@ -887,7 +873,7 @@
         <v>2</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="AA11" s="12"/>
@@ -900,7 +886,7 @@
         <v>10</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -919,12 +905,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -932,12 +918,12 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
@@ -954,7 +940,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="M14" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
@@ -970,7 +956,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1023,7 +1009,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="42">
     <mergeCell ref="M2:U2"/>
     <mergeCell ref="B3:E4"/>
     <mergeCell ref="G3:I3"/>
@@ -1052,9 +1038,8 @@
     <mergeCell ref="U8:AC8"/>
     <mergeCell ref="M9:U9"/>
     <mergeCell ref="D10:G10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="U10:X10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="T10:W10"/>
     <mergeCell ref="AA10:AC10"/>
     <mergeCell ref="J11:N11"/>
     <mergeCell ref="P11:Q11"/>

</xml_diff>

<commit_message>
Inicio de implementação de seleção de gravímetro, a partir de tabela única, para conversão instrumental
</commit_message>
<xml_diff>
--- a/Planejamento da GUI.xlsx
+++ b/Planejamento da GUI.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t xml:space="preserve">Entrada dos dados</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve">______Plan1_____</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N° do Gravímetro:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__996__</t>
   </si>
   <si>
     <t xml:space="preserve">Dados do levantamento</t>
@@ -435,7 +441,7 @@
   <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="AD12" activeCellId="0" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,7 +451,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="2" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="2" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="5.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="2" width="4.71"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,7 +629,7 @@
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -651,11 +659,15 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
-      <c r="T4" s="5"/>
+      <c r="T4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
-      <c r="X4" s="6"/>
+      <c r="X4" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
@@ -669,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
@@ -687,21 +699,21 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="E6" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H6" s="5"/>
       <c r="J6" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -709,7 +721,7 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="U6" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
@@ -731,11 +743,11 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="J7" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K7" s="5"/>
       <c r="M7" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -757,13 +769,13 @@
         <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H8" s="6"/>
       <c r="J8" s="6" t="n">
@@ -771,7 +783,7 @@
       </c>
       <c r="K8" s="6"/>
       <c r="M8" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -779,7 +791,7 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="U8" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="V8" s="9"/>
       <c r="W8" s="9"/>
@@ -795,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -817,19 +829,25 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
       <c r="S10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="T10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
       <c r="X10" s="10"/>
       <c r="AA10" s="10"/>
       <c r="AB10" s="10"/>
@@ -847,7 +865,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -857,7 +875,7 @@
         <v>2</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q11" s="6"/>
       <c r="R11" s="12"/>
@@ -865,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U11" s="6"/>
       <c r="V11" s="12"/>
@@ -873,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y11" s="6"/>
       <c r="AA11" s="12"/>
@@ -886,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
@@ -905,12 +923,12 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
@@ -918,12 +936,12 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
@@ -940,7 +958,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="M14" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
@@ -956,7 +974,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1009,17 +1027,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="44">
     <mergeCell ref="M2:U2"/>
     <mergeCell ref="B3:E4"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:S3"/>
-    <mergeCell ref="T3:W4"/>
-    <mergeCell ref="X3:AC4"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="X3:AC3"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="N4:S4"/>
+    <mergeCell ref="T4:W4"/>
+    <mergeCell ref="X4:AC4"/>
     <mergeCell ref="M5:U5"/>
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="F6:F7"/>

</xml_diff>